<commit_message>
Major fix data-transfer. Additional fix parsing apartments & rentprogress
</commit_message>
<xml_diff>
--- a/src/export_apartment_amenities.xlsx
+++ b/src/export_apartment_amenities.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="125">
   <si>
     <t>'1-Car Garage'</t>
   </si>
@@ -32,36 +32,33 @@
     <t>'Attached Garage'</t>
   </si>
   <si>
-    <t>'Attic'</t>
-  </si>
-  <si>
     <t>'Balcony'</t>
   </si>
   <si>
     <t>'Basement'</t>
   </si>
   <si>
+    <t>'Bathtub w/jets'</t>
+  </si>
+  <si>
     <t>'Bay Window'</t>
   </si>
   <si>
-    <t>'Bike Storage'</t>
-  </si>
-  <si>
     <t>'Bonus Room'</t>
   </si>
   <si>
     <t>'Breakfast Nook'</t>
   </si>
   <si>
+    <t>'Built-In BBQ'</t>
+  </si>
+  <si>
     <t>'Built-In Bookshelves'</t>
   </si>
   <si>
     <t>'Cable Ready'</t>
   </si>
   <si>
-    <t>'Car Charging Station'</t>
-  </si>
-  <si>
     <t>'Carpet'</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>'Coffee System'</t>
   </si>
   <si>
-    <t>'Courtyard'</t>
-  </si>
-  <si>
     <t>'Covered Patio'</t>
   </si>
   <si>
@@ -116,9 +110,6 @@
     <t>'Eat-in Kitchen'</t>
   </si>
   <si>
-    <t>'Elevator'</t>
-  </si>
-  <si>
     <t>'Enclosed Porch / Sunroom'</t>
   </si>
   <si>
@@ -137,9 +128,6 @@
     <t>'Fireplace'</t>
   </si>
   <si>
-    <t>'Fitness Center'</t>
-  </si>
-  <si>
     <t>'Framed Mirrors'</t>
   </si>
   <si>
@@ -170,6 +158,9 @@
     <t>'Great Room'</t>
   </si>
   <si>
+    <t>'Greenhouse'</t>
+  </si>
+  <si>
     <t>'Grill'</t>
   </si>
   <si>
@@ -245,15 +236,12 @@
     <t>'Loft Layout'</t>
   </si>
   <si>
-    <t>'Lounge'</t>
-  </si>
-  <si>
-    <t>'Maid Service'</t>
-  </si>
-  <si>
     <t>'Microwave'</t>
   </si>
   <si>
+    <t>'Mud Room'</t>
+  </si>
+  <si>
     <t>'Natural Light / Sky Lights'</t>
   </si>
   <si>
@@ -275,10 +263,7 @@
     <t>'Patio'</t>
   </si>
   <si>
-    <t>'Pet Door(s)'</t>
-  </si>
-  <si>
-    <t>'Pond'</t>
+    <t>'Plantation Shutters'</t>
   </si>
   <si>
     <t>'Pool'</t>
@@ -293,6 +278,9 @@
     <t>'Range'</t>
   </si>
   <si>
+    <t>'Rear-Loaded Driveway'</t>
+  </si>
+  <si>
     <t>'Recreation Room'</t>
   </si>
   <si>
@@ -302,9 +290,6 @@
     <t>'Satellite TV'</t>
   </si>
   <si>
-    <t>'Sauna'</t>
-  </si>
-  <si>
     <t>'Screened Porch'</t>
   </si>
   <si>
@@ -326,6 +311,9 @@
     <t>'Stainless Steel Appliances'</t>
   </si>
   <si>
+    <t>'Storage Space'</t>
+  </si>
+  <si>
     <t>'Storage Units'</t>
   </si>
   <si>
@@ -335,9 +323,6 @@
     <t>'Surround Sound'</t>
   </si>
   <si>
-    <t>'Tennis Court'</t>
-  </si>
-  <si>
     <t>'Tile Flooring'</t>
   </si>
   <si>
@@ -351,9 +336,6 @@
   </si>
   <si>
     <t>'Tub/Shower'</t>
-  </si>
-  <si>
-    <t>'Vacuum System'</t>
   </si>
   <si>
     <t>'Vaulted Ceiling'</t>
@@ -743,7 +725,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A131"/>
+  <dimension ref="A1:A125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1374,36 +1356,6 @@
     <row r="125" spans="1:1">
       <c r="A125" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1">
-      <c r="A126" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1">
-      <c r="A127" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1">
-      <c r="A128" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1">
-      <c r="A129" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1">
-      <c r="A130" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1">
-      <c r="A131" t="s">
-        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix problems with transferring to WP
</commit_message>
<xml_diff>
--- a/src/export_apartment_amenities.xlsx
+++ b/src/export_apartment_amenities.xlsx
@@ -15,44 +15,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="125">
-  <si>
-    <t>'1-Car Garage'</t>
-  </si>
-  <si>
-    <t>'2-Car Garage'</t>
-  </si>
-  <si>
-    <t>'3-Car Garage'</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
   <si>
     <t>'Air Conditioning'</t>
   </si>
   <si>
-    <t>'Attached Garage'</t>
-  </si>
-  <si>
     <t>'Balcony'</t>
   </si>
   <si>
     <t>'Basement'</t>
   </si>
   <si>
-    <t>'Bathtub w/jets'</t>
-  </si>
-  <si>
-    <t>'Bay Window'</t>
-  </si>
-  <si>
-    <t>'Bonus Room'</t>
-  </si>
-  <si>
     <t>'Breakfast Nook'</t>
   </si>
   <si>
-    <t>'Built-In BBQ'</t>
-  </si>
-  <si>
     <t>'Built-In Bookshelves'</t>
   </si>
   <si>
@@ -62,21 +38,9 @@
     <t>'Carpet'</t>
   </si>
   <si>
-    <t>'Ceiling Fan'</t>
-  </si>
-  <si>
     <t>'Ceiling Fans'</t>
   </si>
   <si>
-    <t>'Central Air/Heat'</t>
-  </si>
-  <si>
-    <t>'Coffee System'</t>
-  </si>
-  <si>
-    <t>'Covered Patio'</t>
-  </si>
-  <si>
     <t>'Crown Molding'</t>
   </si>
   <si>
@@ -104,33 +68,15 @@
     <t>'Double Vanities'</t>
   </si>
   <si>
-    <t>'Dual-Vanity Sinks'</t>
-  </si>
-  <si>
     <t>'Eat-in Kitchen'</t>
   </si>
   <si>
-    <t>'Enclosed Porch / Sunroom'</t>
-  </si>
-  <si>
-    <t>'Extended Driveway'</t>
-  </si>
-  <si>
     <t>'Family Room'</t>
   </si>
   <si>
-    <t>'Fenced Pool'</t>
-  </si>
-  <si>
-    <t>'Fenced Yard'</t>
-  </si>
-  <si>
     <t>'Fireplace'</t>
   </si>
   <si>
-    <t>'Framed Mirrors'</t>
-  </si>
-  <si>
     <t>'Freezer'</t>
   </si>
   <si>
@@ -140,54 +86,27 @@
     <t>'Furnished Units Available'</t>
   </si>
   <si>
-    <t>'Garage'</t>
-  </si>
-  <si>
-    <t>'Garden'</t>
-  </si>
-  <si>
-    <t>'Garden Tub'</t>
-  </si>
-  <si>
     <t>'Gated'</t>
   </si>
   <si>
     <t>'Granite Countertops'</t>
   </si>
   <si>
-    <t>'Great Room'</t>
-  </si>
-  <si>
     <t>'Greenhouse'</t>
   </si>
   <si>
-    <t>'Grill'</t>
-  </si>
-  <si>
     <t>'Handrails'</t>
   </si>
   <si>
-    <t>'Hardwood Flooring'</t>
-  </si>
-  <si>
     <t>'Hardwood Floors'</t>
   </si>
   <si>
     <t>'Heating'</t>
   </si>
   <si>
-    <t>'High Ceilings'</t>
-  </si>
-  <si>
     <t>'High Speed Internet Access'</t>
   </si>
   <si>
-    <t>'Hookup: In-Unit, 1st Floor'</t>
-  </si>
-  <si>
-    <t>'Hookup: In-Unit, 2nd Floor'</t>
-  </si>
-  <si>
     <t>'Ice Maker'</t>
   </si>
   <si>
@@ -206,102 +125,54 @@
     <t>'Kitchen'</t>
   </si>
   <si>
-    <t>'Kitchen Island'</t>
-  </si>
-  <si>
-    <t>'Laminate Flooring'</t>
-  </si>
-  <si>
-    <t>'Large Backyard'</t>
-  </si>
-  <si>
     <t>'Large Bedrooms'</t>
   </si>
   <si>
     <t>'Laundry Facilities'</t>
   </si>
   <si>
-    <t>'Laundry Room'</t>
-  </si>
-  <si>
     <t>'Lawn'</t>
   </si>
   <si>
     <t>'Linen Closet'</t>
   </si>
   <si>
-    <t>'Loft'</t>
-  </si>
-  <si>
     <t>'Loft Layout'</t>
   </si>
   <si>
     <t>'Microwave'</t>
   </si>
   <si>
-    <t>'Mud Room'</t>
-  </si>
-  <si>
-    <t>'Natural Light / Sky Lights'</t>
-  </si>
-  <si>
     <t>'Office'</t>
   </si>
   <si>
-    <t>'Open Floor Plan'</t>
-  </si>
-  <si>
     <t>'Oven'</t>
   </si>
   <si>
-    <t>'Oversized Bathtub'</t>
-  </si>
-  <si>
     <t>'Pantry'</t>
   </si>
   <si>
     <t>'Patio'</t>
   </si>
   <si>
-    <t>'Plantation Shutters'</t>
-  </si>
-  <si>
-    <t>'Pool'</t>
+    <t>'Playground'</t>
   </si>
   <si>
     <t>'Porch'</t>
   </si>
   <si>
-    <t>'Quartz Countertops'</t>
-  </si>
-  <si>
     <t>'Range'</t>
   </si>
   <si>
-    <t>'Rear-Loaded Driveway'</t>
-  </si>
-  <si>
-    <t>'Recreation Room'</t>
-  </si>
-  <si>
     <t>'Refrigerator'</t>
   </si>
   <si>
-    <t>'Satellite TV'</t>
-  </si>
-  <si>
-    <t>'Screened Porch'</t>
-  </si>
-  <si>
     <t>'Security System'</t>
   </si>
   <si>
     <t>'Skylight'</t>
   </si>
   <si>
-    <t>'Smart Home'</t>
-  </si>
-  <si>
     <t>'Smoke Free'</t>
   </si>
   <si>
@@ -311,30 +182,18 @@
     <t>'Stainless Steel Appliances'</t>
   </si>
   <si>
-    <t>'Storage Space'</t>
-  </si>
-  <si>
     <t>'Storage Units'</t>
   </si>
   <si>
     <t>'Sunroom'</t>
   </si>
   <si>
-    <t>'Surround Sound'</t>
-  </si>
-  <si>
-    <t>'Tile Flooring'</t>
-  </si>
-  <si>
     <t>'Tile Floors'</t>
   </si>
   <si>
     <t>'Trash Compactor'</t>
   </si>
   <si>
-    <t>'Travertine Flooring'</t>
-  </si>
-  <si>
     <t>'Tub/Shower'</t>
   </si>
   <si>
@@ -347,27 +206,9 @@
     <t>'Vinyl Flooring'</t>
   </si>
   <si>
-    <t>'Vinyl Plank Flooring'</t>
-  </si>
-  <si>
-    <t>'Walk-In Closet'</t>
-  </si>
-  <si>
     <t>'Walk-In Closets'</t>
   </si>
   <si>
-    <t>'Walk-In Pantry'</t>
-  </si>
-  <si>
-    <t>'Walk-In Shower'</t>
-  </si>
-  <si>
-    <t>'Wall Oven'</t>
-  </si>
-  <si>
-    <t>'Warming Drawer'</t>
-  </si>
-  <si>
     <t>'Washer/Dryer Hookup'</t>
   </si>
   <si>
@@ -381,12 +222,6 @@
   </si>
   <si>
     <t>'Window Coverings'</t>
-  </si>
-  <si>
-    <t>'Wood Fireplace'</t>
-  </si>
-  <si>
-    <t>'Wood-Look Blinds'</t>
   </si>
   <si>
     <t>'Yard'</t>
@@ -725,7 +560,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A125"/>
+  <dimension ref="A1:A70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1081,281 +916,6 @@
     <row r="70" spans="1:1">
       <c r="A70" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1">
-      <c r="A74" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1">
-      <c r="A75" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1">
-      <c r="A76" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1">
-      <c r="A78" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1">
-      <c r="A79" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1">
-      <c r="A80" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1">
-      <c r="A81" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1">
-      <c r="A82" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1">
-      <c r="A83" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1">
-      <c r="A84" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1">
-      <c r="A85" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1">
-      <c r="A86" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1">
-      <c r="A87" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1">
-      <c r="A88" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1">
-      <c r="A89" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1">
-      <c r="A90" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1">
-      <c r="A91" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1">
-      <c r="A92" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1">
-      <c r="A93" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1">
-      <c r="A94" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1">
-      <c r="A95" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1">
-      <c r="A96" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1">
-      <c r="A97" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1">
-      <c r="A98" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1">
-      <c r="A99" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1">
-      <c r="A100" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1">
-      <c r="A101" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1">
-      <c r="A102" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1">
-      <c r="A103" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1">
-      <c r="A104" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1">
-      <c r="A105" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1">
-      <c r="A106" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1">
-      <c r="A107" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1">
-      <c r="A108" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1">
-      <c r="A109" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1">
-      <c r="A110" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1">
-      <c r="A111" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1">
-      <c r="A112" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1">
-      <c r="A113" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1">
-      <c r="A114" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1">
-      <c r="A115" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1">
-      <c r="A116" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1">
-      <c r="A117" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1">
-      <c r="A118" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1">
-      <c r="A119" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1">
-      <c r="A120" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1">
-      <c r="A121" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1">
-      <c r="A122" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1">
-      <c r="A123" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1">
-      <c r="A124" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1">
-      <c r="A125" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>